<commit_message>
stu2 docs update 3
</commit_message>
<xml_diff>
--- a/docs/ValueSet-ValueSet-apgar-timing.xlsx
+++ b/docs/ValueSet-ValueSet-apgar-timing.xlsx
@@ -43,7 +43,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>ValueSet - APGAR Score Timing</t>
+    <t>APGAR Score Timing</t>
   </si>
   <si>
     <t>Status</t>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-13T11:56:10-05:00</t>
+    <t>2024-02-27T09:44:15-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>